<commit_message>
fix upload xls for kyca,add 10 po
</commit_message>
<xml_diff>
--- a/FrmPIE/0temple/templesforKYCA.xlsx
+++ b/FrmPIE/0temple/templesforKYCA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="102">
   <si>
     <t>Supplier Inv no.</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>10736367</t>
-  </si>
-  <si>
-    <t>75000</t>
   </si>
   <si>
     <t>7LCQ670181S+H01</t>
@@ -292,6 +289,7 @@
       <rPr>
         <sz val="9"/>
         <rFont val="宋体"/>
+        <charset val="134"/>
       </rPr>
       <t>85</t>
     </r>
@@ -302,6 +300,164 @@
         <charset val="134"/>
       </rPr>
       <t>-686</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PO7</t>
+  </si>
+  <si>
+    <t>QTY7</t>
+  </si>
+  <si>
+    <t>PO8</t>
+  </si>
+  <si>
+    <t>QTY8</t>
+  </si>
+  <si>
+    <t>PO9</t>
+  </si>
+  <si>
+    <t>QTY9</t>
+  </si>
+  <si>
+    <t>PO10</t>
+  </si>
+  <si>
+    <t>QTY10</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1-10</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -659,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -672,7 +828,7 @@
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,8 +889,34 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -796,7 +978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -834,10 +1016,10 @@
         <v>45</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>46</v>
@@ -851,14 +1033,8 @@
       <c r="R3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:30">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -920,7 +1096,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:30">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -982,7 +1158,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:30">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1044,7 +1220,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1055,7 +1231,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
@@ -1072,14 +1248,14 @@
       <c r="I7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>74</v>
+      <c r="J7" s="1">
+        <v>70000</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
+      </c>
+      <c r="L7" s="1">
+        <v>5000</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>46</v>
@@ -1106,39 +1282,39 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:30">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="L8" s="1">
         <v>3000</v>
@@ -1167,6 +1343,94 @@
       <c r="T8" s="1" t="s">
         <v>46</v>
       </c>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1">
+        <v>55</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="N9" s="1">
+        <v>3</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="P9" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="R9" s="1">
+        <v>5</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="T9" s="1">
+        <v>6</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V9" s="1">
+        <v>7</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="X9" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fix add avg for upload kyca
</commit_message>
<xml_diff>
--- a/FrmPIE/0temple/templesforKYCA.xlsx
+++ b/FrmPIE/0temple/templesforKYCA.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\0work\2014\gitpie\FrmPIE\0temple\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14715" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="0105凎嚙螔嫟2" sheetId="1" r:id="rId1"/>
+    <sheet name="0105" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'0105凎嚙螔嫟2'!$A$1:$T$142</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'0105凎嚙螔嫟2'!$1:$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'0105'!$A$1:$T$142</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'0105'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="410">
   <si>
     <t>7YCS12B1008+H01</t>
   </si>
@@ -1255,11 +1261,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="188" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="176" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -1340,10 +1346,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1352,7 +1358,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1364,7 +1370,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1376,7 +1382,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1397,7 +1403,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1406,6 +1412,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1452,7 +1466,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1484,9 +1498,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1518,6 +1533,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1693,14 +1709,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" style="1" bestFit="1" customWidth="1"/>
@@ -1725,7 +1741,7 @@
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>400</v>
       </c>
@@ -1783,7 +1799,7 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="49.5" customHeight="1">
+    <row r="2" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>401</v>
       </c>
@@ -1831,7 +1847,7 @@
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
     </row>
-    <row r="3" spans="1:20" ht="49.5" customHeight="1">
+    <row r="3" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>401</v>
       </c>
@@ -1871,7 +1887,7 @@
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
     </row>
-    <row r="4" spans="1:20" ht="49.5" customHeight="1">
+    <row r="4" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>401</v>
       </c>
@@ -1915,7 +1931,7 @@
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="49.5" customHeight="1">
+    <row r="5" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>401</v>
       </c>
@@ -1959,7 +1975,7 @@
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="6" spans="1:20" ht="49.5" customHeight="1">
+    <row r="6" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>401</v>
       </c>
@@ -2007,7 +2023,7 @@
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
     </row>
-    <row r="7" spans="1:20" ht="49.5" customHeight="1">
+    <row r="7" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>401</v>
       </c>
@@ -2051,7 +2067,7 @@
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
     </row>
-    <row r="8" spans="1:20" ht="49.5" customHeight="1">
+    <row r="8" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>401</v>
       </c>
@@ -2099,7 +2115,7 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="49.5" customHeight="1">
+    <row r="9" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>401</v>
       </c>
@@ -2143,7 +2159,7 @@
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="10" spans="1:20" ht="49.5" customHeight="1">
+    <row r="10" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>401</v>
       </c>
@@ -2187,7 +2203,7 @@
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
     </row>
-    <row r="11" spans="1:20" ht="49.5" customHeight="1">
+    <row r="11" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>401</v>
       </c>
@@ -2235,7 +2251,7 @@
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
     </row>
-    <row r="12" spans="1:20" ht="49.5" customHeight="1">
+    <row r="12" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>401</v>
       </c>
@@ -2283,7 +2299,7 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
     </row>
-    <row r="13" spans="1:20" ht="49.5" customHeight="1">
+    <row r="13" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>401</v>
       </c>
@@ -2323,7 +2339,7 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
     </row>
-    <row r="14" spans="1:20" ht="49.5" customHeight="1">
+    <row r="14" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>401</v>
       </c>
@@ -2363,7 +2379,7 @@
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
     </row>
-    <row r="15" spans="1:20" ht="49.5" customHeight="1">
+    <row r="15" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>401</v>
       </c>
@@ -2403,7 +2419,7 @@
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
     </row>
-    <row r="16" spans="1:20" ht="49.5" customHeight="1">
+    <row r="16" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
         <v>401</v>
       </c>
@@ -2447,7 +2463,7 @@
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
     </row>
-    <row r="17" spans="1:18" ht="49.5" customHeight="1">
+    <row r="17" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
         <v>401</v>
       </c>
@@ -2495,7 +2511,7 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="1:18" ht="49.5" customHeight="1">
+    <row r="18" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
         <v>401</v>
       </c>
@@ -2539,7 +2555,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="1:18" ht="49.5" customHeight="1">
+    <row r="19" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
         <v>401</v>
       </c>
@@ -2583,7 +2599,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18" ht="49.5" customHeight="1">
+    <row r="20" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
         <v>401</v>
       </c>
@@ -2627,7 +2643,7 @@
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:18" ht="49.5" customHeight="1">
+    <row r="21" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
         <v>401</v>
       </c>
@@ -2671,7 +2687,7 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:18" ht="49.5" customHeight="1">
+    <row r="22" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>401</v>
       </c>
@@ -2715,7 +2731,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:18" ht="49.5" customHeight="1">
+    <row r="23" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
         <v>401</v>
       </c>
@@ -2759,7 +2775,7 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:18" ht="49.5" customHeight="1">
+    <row r="24" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
         <v>401</v>
       </c>
@@ -2803,7 +2819,7 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:18" ht="49.5" customHeight="1">
+    <row r="25" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
         <v>401</v>
       </c>
@@ -2855,7 +2871,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:18" ht="49.5" customHeight="1">
+    <row r="26" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
         <v>401</v>
       </c>
@@ -2895,7 +2911,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18" ht="49.5" customHeight="1">
+    <row r="27" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
         <v>401</v>
       </c>
@@ -2939,7 +2955,7 @@
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
     </row>
-    <row r="28" spans="1:18" ht="49.5" customHeight="1">
+    <row r="28" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
         <v>401</v>
       </c>
@@ -2979,7 +2995,7 @@
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
     </row>
-    <row r="29" spans="1:18" ht="49.5" customHeight="1">
+    <row r="29" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
         <v>401</v>
       </c>
@@ -3027,7 +3043,7 @@
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
     </row>
-    <row r="30" spans="1:18" ht="49.5" customHeight="1">
+    <row r="30" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="s">
         <v>401</v>
       </c>
@@ -3075,7 +3091,7 @@
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
     </row>
-    <row r="31" spans="1:18" ht="49.5" customHeight="1">
+    <row r="31" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
         <v>401</v>
       </c>
@@ -3119,7 +3135,7 @@
       <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
     </row>
-    <row r="32" spans="1:18" ht="49.5" customHeight="1">
+    <row r="32" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
         <v>401</v>
       </c>
@@ -3163,7 +3179,7 @@
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
     </row>
-    <row r="33" spans="1:18" ht="49.5" customHeight="1">
+    <row r="33" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="s">
         <v>401</v>
       </c>
@@ -3207,7 +3223,7 @@
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
     </row>
-    <row r="34" spans="1:18" ht="49.5" customHeight="1">
+    <row r="34" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="12" t="s">
         <v>401</v>
       </c>
@@ -3251,7 +3267,7 @@
       <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
     </row>
-    <row r="35" spans="1:18" ht="49.5" customHeight="1">
+    <row r="35" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
         <v>401</v>
       </c>
@@ -3295,7 +3311,7 @@
       <c r="Q35" s="15"/>
       <c r="R35" s="15"/>
     </row>
-    <row r="36" spans="1:18" ht="49.5" customHeight="1">
+    <row r="36" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
         <v>401</v>
       </c>
@@ -3343,7 +3359,7 @@
       <c r="Q36" s="15"/>
       <c r="R36" s="15"/>
     </row>
-    <row r="37" spans="1:18" ht="49.5" customHeight="1">
+    <row r="37" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="12" t="s">
         <v>401</v>
       </c>
@@ -3391,7 +3407,7 @@
       <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
     </row>
-    <row r="38" spans="1:18" ht="49.5" customHeight="1">
+    <row r="38" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="12" t="s">
         <v>401</v>
       </c>
@@ -3439,7 +3455,7 @@
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
     </row>
-    <row r="39" spans="1:18" ht="49.5" customHeight="1">
+    <row r="39" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="s">
         <v>401</v>
       </c>
@@ -3487,7 +3503,7 @@
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
     </row>
-    <row r="40" spans="1:18" ht="49.5" customHeight="1">
+    <row r="40" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="12" t="s">
         <v>401</v>
       </c>
@@ -3531,7 +3547,7 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
     </row>
-    <row r="41" spans="1:18" ht="49.5" customHeight="1">
+    <row r="41" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="12" t="s">
         <v>401</v>
       </c>
@@ -3579,7 +3595,7 @@
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
     </row>
-    <row r="42" spans="1:18" ht="49.5" customHeight="1">
+    <row r="42" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="12" t="s">
         <v>401</v>
       </c>
@@ -3623,7 +3639,7 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
     </row>
-    <row r="43" spans="1:18" ht="49.5" customHeight="1">
+    <row r="43" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="12" t="s">
         <v>401</v>
       </c>
@@ -3671,7 +3687,7 @@
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
     </row>
-    <row r="44" spans="1:18" ht="49.5" customHeight="1">
+    <row r="44" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="12" t="s">
         <v>401</v>
       </c>
@@ -3711,7 +3727,7 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
     </row>
-    <row r="45" spans="1:18" ht="49.5" customHeight="1">
+    <row r="45" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="12" t="s">
         <v>401</v>
       </c>
@@ -3755,7 +3771,7 @@
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
     </row>
-    <row r="46" spans="1:18" ht="49.5" customHeight="1">
+    <row r="46" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="12" t="s">
         <v>401</v>
       </c>
@@ -3803,7 +3819,7 @@
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
     </row>
-    <row r="47" spans="1:18" ht="49.5" customHeight="1">
+    <row r="47" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
         <v>401</v>
       </c>
@@ -3843,7 +3859,7 @@
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
     </row>
-    <row r="48" spans="1:18" ht="49.5" customHeight="1">
+    <row r="48" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="12" t="s">
         <v>401</v>
       </c>
@@ -3883,7 +3899,7 @@
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
     </row>
-    <row r="49" spans="1:18" ht="49.5" customHeight="1">
+    <row r="49" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="12" t="s">
         <v>401</v>
       </c>
@@ -3927,7 +3943,7 @@
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
     </row>
-    <row r="50" spans="1:18" ht="49.5" customHeight="1">
+    <row r="50" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="12" t="s">
         <v>401</v>
       </c>
@@ -3971,7 +3987,7 @@
       <c r="Q50" s="15"/>
       <c r="R50" s="15"/>
     </row>
-    <row r="51" spans="1:18" ht="49.5" customHeight="1">
+    <row r="51" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="12" t="s">
         <v>401</v>
       </c>
@@ -4015,7 +4031,7 @@
       <c r="Q51" s="15"/>
       <c r="R51" s="15"/>
     </row>
-    <row r="52" spans="1:18" ht="49.5" customHeight="1">
+    <row r="52" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="12" t="s">
         <v>401</v>
       </c>
@@ -4059,7 +4075,7 @@
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
     </row>
-    <row r="53" spans="1:18" ht="49.5" customHeight="1">
+    <row r="53" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="12" t="s">
         <v>401</v>
       </c>
@@ -4103,7 +4119,7 @@
       <c r="Q53" s="15"/>
       <c r="R53" s="15"/>
     </row>
-    <row r="54" spans="1:18" ht="49.5" customHeight="1">
+    <row r="54" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="s">
         <v>401</v>
       </c>
@@ -4151,7 +4167,7 @@
       <c r="Q54" s="15"/>
       <c r="R54" s="15"/>
     </row>
-    <row r="55" spans="1:18" ht="49.5" customHeight="1">
+    <row r="55" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="12" t="s">
         <v>401</v>
       </c>
@@ -4203,7 +4219,7 @@
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
     </row>
-    <row r="56" spans="1:18" ht="49.5" customHeight="1">
+    <row r="56" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="12" t="s">
         <v>401</v>
       </c>
@@ -4243,7 +4259,7 @@
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
     </row>
-    <row r="57" spans="1:18" ht="49.5" customHeight="1">
+    <row r="57" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="12" t="s">
         <v>401</v>
       </c>
@@ -4291,7 +4307,7 @@
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
     </row>
-    <row r="58" spans="1:18" ht="49.5" customHeight="1">
+    <row r="58" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="12" t="s">
         <v>401</v>
       </c>
@@ -4339,7 +4355,7 @@
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
     </row>
-    <row r="59" spans="1:18" ht="49.5" customHeight="1">
+    <row r="59" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="12" t="s">
         <v>401</v>
       </c>
@@ -4383,7 +4399,7 @@
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
     </row>
-    <row r="60" spans="1:18" ht="49.5" customHeight="1">
+    <row r="60" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="12" t="s">
         <v>401</v>
       </c>
@@ -4423,7 +4439,7 @@
       <c r="Q60" s="15"/>
       <c r="R60" s="15"/>
     </row>
-    <row r="61" spans="1:18" ht="49.5" customHeight="1">
+    <row r="61" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="12" t="s">
         <v>401</v>
       </c>
@@ -4463,7 +4479,7 @@
       <c r="Q61" s="15"/>
       <c r="R61" s="15"/>
     </row>
-    <row r="62" spans="1:18" ht="49.5" customHeight="1">
+    <row r="62" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="12" t="s">
         <v>401</v>
       </c>
@@ -4519,7 +4535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="49.5" customHeight="1">
+    <row r="63" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="12" t="s">
         <v>401</v>
       </c>
@@ -4559,7 +4575,7 @@
       <c r="Q63" s="15"/>
       <c r="R63" s="15"/>
     </row>
-    <row r="64" spans="1:18" ht="49.5" customHeight="1">
+    <row r="64" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="12" t="s">
         <v>401</v>
       </c>
@@ -4603,7 +4619,7 @@
       <c r="Q64" s="15"/>
       <c r="R64" s="15"/>
     </row>
-    <row r="65" spans="1:18" ht="49.5" customHeight="1">
+    <row r="65" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="12" t="s">
         <v>401</v>
       </c>
@@ -4647,7 +4663,7 @@
       <c r="Q65" s="15"/>
       <c r="R65" s="15"/>
     </row>
-    <row r="66" spans="1:18" ht="49.5" customHeight="1">
+    <row r="66" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="12" t="s">
         <v>401</v>
       </c>
@@ -4691,7 +4707,7 @@
       <c r="Q66" s="15"/>
       <c r="R66" s="15"/>
     </row>
-    <row r="67" spans="1:18" ht="49.5" customHeight="1">
+    <row r="67" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="12" t="s">
         <v>401</v>
       </c>
@@ -4731,7 +4747,7 @@
       <c r="Q67" s="15"/>
       <c r="R67" s="15"/>
     </row>
-    <row r="68" spans="1:18" ht="49.5" customHeight="1">
+    <row r="68" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="12" t="s">
         <v>401</v>
       </c>
@@ -4775,7 +4791,7 @@
       <c r="Q68" s="15"/>
       <c r="R68" s="15"/>
     </row>
-    <row r="69" spans="1:18" ht="49.5" customHeight="1">
+    <row r="69" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="12" t="s">
         <v>401</v>
       </c>
@@ -4819,7 +4835,7 @@
       <c r="Q69" s="15"/>
       <c r="R69" s="15"/>
     </row>
-    <row r="70" spans="1:18" ht="49.5" customHeight="1">
+    <row r="70" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="12" t="s">
         <v>401</v>
       </c>
@@ -4867,7 +4883,7 @@
       <c r="Q70" s="15"/>
       <c r="R70" s="15"/>
     </row>
-    <row r="71" spans="1:18" ht="49.5" customHeight="1">
+    <row r="71" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="12" t="s">
         <v>401</v>
       </c>
@@ -4907,7 +4923,7 @@
       <c r="Q71" s="15"/>
       <c r="R71" s="15"/>
     </row>
-    <row r="72" spans="1:18" ht="49.5" customHeight="1">
+    <row r="72" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="12" t="s">
         <v>401</v>
       </c>
@@ -4951,7 +4967,7 @@
       <c r="Q72" s="15"/>
       <c r="R72" s="15"/>
     </row>
-    <row r="73" spans="1:18" ht="49.5" customHeight="1">
+    <row r="73" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="12" t="s">
         <v>401</v>
       </c>
@@ -4999,7 +5015,7 @@
       <c r="Q73" s="15"/>
       <c r="R73" s="15"/>
     </row>
-    <row r="74" spans="1:18" ht="49.5" customHeight="1">
+    <row r="74" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="12" t="s">
         <v>401</v>
       </c>
@@ -5043,7 +5059,7 @@
       <c r="Q74" s="15"/>
       <c r="R74" s="15"/>
     </row>
-    <row r="75" spans="1:18" ht="49.5" customHeight="1">
+    <row r="75" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="12" t="s">
         <v>401</v>
       </c>
@@ -5087,7 +5103,7 @@
       <c r="Q75" s="15"/>
       <c r="R75" s="15"/>
     </row>
-    <row r="76" spans="1:18" ht="49.5" customHeight="1">
+    <row r="76" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="12" t="s">
         <v>401</v>
       </c>
@@ -5131,7 +5147,7 @@
       <c r="Q76" s="15"/>
       <c r="R76" s="15"/>
     </row>
-    <row r="77" spans="1:18" ht="49.5" customHeight="1">
+    <row r="77" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="12" t="s">
         <v>401</v>
       </c>
@@ -5175,7 +5191,7 @@
       <c r="Q77" s="15"/>
       <c r="R77" s="15"/>
     </row>
-    <row r="78" spans="1:18" ht="49.5" customHeight="1">
+    <row r="78" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="12" t="s">
         <v>401</v>
       </c>
@@ -5219,7 +5235,7 @@
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
     </row>
-    <row r="79" spans="1:18" ht="49.5" customHeight="1">
+    <row r="79" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="12" t="s">
         <v>401</v>
       </c>
@@ -5267,7 +5283,7 @@
       <c r="Q79" s="15"/>
       <c r="R79" s="15"/>
     </row>
-    <row r="80" spans="1:18" ht="49.5" customHeight="1">
+    <row r="80" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="12" t="s">
         <v>401</v>
       </c>
@@ -5307,7 +5323,7 @@
       <c r="Q80" s="15"/>
       <c r="R80" s="15"/>
     </row>
-    <row r="81" spans="1:18" ht="49.5" customHeight="1">
+    <row r="81" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="12" t="s">
         <v>401</v>
       </c>
@@ -5351,7 +5367,7 @@
       <c r="Q81" s="15"/>
       <c r="R81" s="15"/>
     </row>
-    <row r="82" spans="1:18" ht="49.5" customHeight="1">
+    <row r="82" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="12" t="s">
         <v>401</v>
       </c>
@@ -5399,7 +5415,7 @@
       <c r="Q82" s="15"/>
       <c r="R82" s="15"/>
     </row>
-    <row r="83" spans="1:18" ht="49.5" customHeight="1">
+    <row r="83" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="12" t="s">
         <v>401</v>
       </c>
@@ -5443,7 +5459,7 @@
       <c r="Q83" s="15"/>
       <c r="R83" s="15"/>
     </row>
-    <row r="84" spans="1:18" ht="49.5" customHeight="1">
+    <row r="84" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="12" t="s">
         <v>401</v>
       </c>
@@ -5487,7 +5503,7 @@
       <c r="Q84" s="15"/>
       <c r="R84" s="15"/>
     </row>
-    <row r="85" spans="1:18" ht="49.5" customHeight="1">
+    <row r="85" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="12" t="s">
         <v>401</v>
       </c>
@@ -5527,7 +5543,7 @@
       <c r="Q85" s="15"/>
       <c r="R85" s="15"/>
     </row>
-    <row r="86" spans="1:18" ht="49.5" customHeight="1">
+    <row r="86" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="12" t="s">
         <v>401</v>
       </c>
@@ -5575,7 +5591,7 @@
       <c r="Q86" s="15"/>
       <c r="R86" s="15"/>
     </row>
-    <row r="87" spans="1:18" ht="49.5" customHeight="1">
+    <row r="87" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="12" t="s">
         <v>401</v>
       </c>
@@ -5615,7 +5631,7 @@
       <c r="Q87" s="15"/>
       <c r="R87" s="15"/>
     </row>
-    <row r="88" spans="1:18" ht="49.5" customHeight="1">
+    <row r="88" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="12" t="s">
         <v>401</v>
       </c>
@@ -5659,7 +5675,7 @@
       <c r="Q88" s="15"/>
       <c r="R88" s="15"/>
     </row>
-    <row r="89" spans="1:18" ht="49.5" customHeight="1">
+    <row r="89" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="12" t="s">
         <v>401</v>
       </c>
@@ -5703,7 +5719,7 @@
       <c r="Q89" s="15"/>
       <c r="R89" s="15"/>
     </row>
-    <row r="90" spans="1:18" ht="49.5" customHeight="1">
+    <row r="90" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="12" t="s">
         <v>401</v>
       </c>
@@ -5747,7 +5763,7 @@
       <c r="Q90" s="15"/>
       <c r="R90" s="15"/>
     </row>
-    <row r="91" spans="1:18" ht="49.5" customHeight="1">
+    <row r="91" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="12" t="s">
         <v>401</v>
       </c>
@@ -5787,7 +5803,7 @@
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
     </row>
-    <row r="92" spans="1:18" ht="49.5" customHeight="1">
+    <row r="92" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="12" t="s">
         <v>401</v>
       </c>
@@ -5835,7 +5851,7 @@
       <c r="Q92" s="15"/>
       <c r="R92" s="15"/>
     </row>
-    <row r="93" spans="1:18" ht="49.5" customHeight="1">
+    <row r="93" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="12" t="s">
         <v>401</v>
       </c>
@@ -5879,7 +5895,7 @@
       <c r="Q93" s="15"/>
       <c r="R93" s="15"/>
     </row>
-    <row r="94" spans="1:18" ht="49.5" customHeight="1">
+    <row r="94" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="12" t="s">
         <v>401</v>
       </c>
@@ -5919,7 +5935,7 @@
       <c r="Q94" s="15"/>
       <c r="R94" s="15"/>
     </row>
-    <row r="95" spans="1:18" ht="49.5" customHeight="1">
+    <row r="95" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="12" t="s">
         <v>401</v>
       </c>
@@ -5963,7 +5979,7 @@
       <c r="Q95" s="15"/>
       <c r="R95" s="15"/>
     </row>
-    <row r="96" spans="1:18" ht="49.5" customHeight="1">
+    <row r="96" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="12" t="s">
         <v>401</v>
       </c>
@@ -6007,7 +6023,7 @@
       <c r="Q96" s="15"/>
       <c r="R96" s="15"/>
     </row>
-    <row r="97" spans="1:18" ht="49.5" customHeight="1">
+    <row r="97" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="12" t="s">
         <v>401</v>
       </c>
@@ -6051,7 +6067,7 @@
       <c r="Q97" s="15"/>
       <c r="R97" s="15"/>
     </row>
-    <row r="98" spans="1:18" ht="49.5" customHeight="1">
+    <row r="98" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="12" t="s">
         <v>401</v>
       </c>
@@ -6099,7 +6115,7 @@
       <c r="Q98" s="15"/>
       <c r="R98" s="15"/>
     </row>
-    <row r="99" spans="1:18" ht="49.5" customHeight="1">
+    <row r="99" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="12" t="s">
         <v>401</v>
       </c>
@@ -6139,7 +6155,7 @@
       <c r="Q99" s="15"/>
       <c r="R99" s="15"/>
     </row>
-    <row r="100" spans="1:18" ht="49.5" customHeight="1">
+    <row r="100" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="12" t="s">
         <v>401</v>
       </c>
@@ -6183,7 +6199,7 @@
       <c r="Q100" s="15"/>
       <c r="R100" s="15"/>
     </row>
-    <row r="101" spans="1:18" ht="49.5" customHeight="1">
+    <row r="101" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="12" t="s">
         <v>401</v>
       </c>
@@ -6223,7 +6239,7 @@
       <c r="Q101" s="15"/>
       <c r="R101" s="15"/>
     </row>
-    <row r="102" spans="1:18" ht="49.5" customHeight="1">
+    <row r="102" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="12" t="s">
         <v>401</v>
       </c>
@@ -6263,7 +6279,7 @@
       <c r="Q102" s="15"/>
       <c r="R102" s="15"/>
     </row>
-    <row r="103" spans="1:18" ht="49.5" customHeight="1">
+    <row r="103" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="12" t="s">
         <v>401</v>
       </c>
@@ -6303,7 +6319,7 @@
       <c r="Q103" s="15"/>
       <c r="R103" s="15"/>
     </row>
-    <row r="104" spans="1:18" ht="49.5" customHeight="1">
+    <row r="104" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="12" t="s">
         <v>401</v>
       </c>
@@ -6343,7 +6359,7 @@
       <c r="Q104" s="15"/>
       <c r="R104" s="15"/>
     </row>
-    <row r="105" spans="1:18" ht="49.5" customHeight="1">
+    <row r="105" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="12" t="s">
         <v>401</v>
       </c>
@@ -6383,7 +6399,7 @@
       <c r="Q105" s="15"/>
       <c r="R105" s="15"/>
     </row>
-    <row r="106" spans="1:18" ht="49.5" customHeight="1">
+    <row r="106" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="12" t="s">
         <v>401</v>
       </c>
@@ -6423,7 +6439,7 @@
       <c r="Q106" s="15"/>
       <c r="R106" s="15"/>
     </row>
-    <row r="107" spans="1:18" ht="49.5" customHeight="1">
+    <row r="107" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="12" t="s">
         <v>401</v>
       </c>
@@ -6467,7 +6483,7 @@
       <c r="Q107" s="15"/>
       <c r="R107" s="15"/>
     </row>
-    <row r="108" spans="1:18" ht="49.5" customHeight="1">
+    <row r="108" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="12" t="s">
         <v>401</v>
       </c>
@@ -6507,7 +6523,7 @@
       <c r="Q108" s="15"/>
       <c r="R108" s="15"/>
     </row>
-    <row r="109" spans="1:18" ht="49.5" customHeight="1">
+    <row r="109" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="12" t="s">
         <v>401</v>
       </c>
@@ -6547,7 +6563,7 @@
       <c r="Q109" s="15"/>
       <c r="R109" s="15"/>
     </row>
-    <row r="110" spans="1:18" ht="49.5" customHeight="1">
+    <row r="110" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="12" t="s">
         <v>401</v>
       </c>
@@ -6591,7 +6607,7 @@
       <c r="Q110" s="15"/>
       <c r="R110" s="15"/>
     </row>
-    <row r="111" spans="1:18" ht="49.5" customHeight="1">
+    <row r="111" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="12" t="s">
         <v>401</v>
       </c>
@@ -6639,7 +6655,7 @@
       <c r="Q111" s="15"/>
       <c r="R111" s="15"/>
     </row>
-    <row r="112" spans="1:18" ht="49.5" customHeight="1">
+    <row r="112" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="12" t="s">
         <v>401</v>
       </c>
@@ -6683,7 +6699,7 @@
       <c r="Q112" s="15"/>
       <c r="R112" s="15"/>
     </row>
-    <row r="113" spans="1:18" ht="49.5" customHeight="1">
+    <row r="113" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="12" t="s">
         <v>401</v>
       </c>
@@ -6727,7 +6743,7 @@
       <c r="Q113" s="15"/>
       <c r="R113" s="15"/>
     </row>
-    <row r="114" spans="1:18" ht="49.5" customHeight="1">
+    <row r="114" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="12" t="s">
         <v>401</v>
       </c>
@@ -6771,7 +6787,7 @@
       <c r="Q114" s="15"/>
       <c r="R114" s="15"/>
     </row>
-    <row r="115" spans="1:18" ht="49.5" customHeight="1">
+    <row r="115" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="12" t="s">
         <v>401</v>
       </c>
@@ -6815,7 +6831,7 @@
       <c r="Q115" s="15"/>
       <c r="R115" s="15"/>
     </row>
-    <row r="116" spans="1:18" ht="49.5" customHeight="1">
+    <row r="116" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="12" t="s">
         <v>401</v>
       </c>
@@ -6863,7 +6879,7 @@
       <c r="Q116" s="15"/>
       <c r="R116" s="15"/>
     </row>
-    <row r="117" spans="1:18" ht="49.5" customHeight="1">
+    <row r="117" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="12" t="s">
         <v>401</v>
       </c>
@@ -6903,7 +6919,7 @@
       <c r="Q117" s="15"/>
       <c r="R117" s="15"/>
     </row>
-    <row r="118" spans="1:18" ht="49.5" customHeight="1" thickBot="1">
+    <row r="118" spans="1:18" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A118" s="12" t="s">
         <v>401</v>
       </c>
@@ -6947,7 +6963,7 @@
       <c r="Q118" s="15"/>
       <c r="R118" s="15"/>
     </row>
-    <row r="119" spans="1:18" ht="49.5" customHeight="1" thickBot="1">
+    <row r="119" spans="1:18" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="s">
         <v>401</v>
       </c>
@@ -6995,7 +7011,7 @@
       <c r="Q119" s="15"/>
       <c r="R119" s="15"/>
     </row>
-    <row r="120" spans="1:18" ht="49.5" customHeight="1" thickBot="1">
+    <row r="120" spans="1:18" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="s">
         <v>401</v>
       </c>
@@ -7043,7 +7059,7 @@
       <c r="Q120" s="15"/>
       <c r="R120" s="15"/>
     </row>
-    <row r="121" spans="1:18" ht="49.5" customHeight="1">
+    <row r="121" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="12" t="s">
         <v>401</v>
       </c>
@@ -7087,7 +7103,7 @@
       <c r="Q121" s="15"/>
       <c r="R121" s="15"/>
     </row>
-    <row r="122" spans="1:18" ht="49.5" customHeight="1">
+    <row r="122" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="12" t="s">
         <v>401</v>
       </c>
@@ -7131,7 +7147,7 @@
       <c r="Q122" s="15"/>
       <c r="R122" s="15"/>
     </row>
-    <row r="123" spans="1:18" ht="49.5" customHeight="1">
+    <row r="123" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="12" t="s">
         <v>401</v>
       </c>
@@ -7175,7 +7191,7 @@
       <c r="Q123" s="15"/>
       <c r="R123" s="15"/>
     </row>
-    <row r="124" spans="1:18" ht="49.5" customHeight="1">
+    <row r="124" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="12" t="s">
         <v>401</v>
       </c>
@@ -7219,7 +7235,7 @@
       <c r="Q124" s="15"/>
       <c r="R124" s="15"/>
     </row>
-    <row r="125" spans="1:18" ht="49.5" customHeight="1">
+    <row r="125" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="12" t="s">
         <v>401</v>
       </c>
@@ -7267,7 +7283,7 @@
       <c r="Q125" s="15"/>
       <c r="R125" s="15"/>
     </row>
-    <row r="126" spans="1:18" ht="49.5" customHeight="1">
+    <row r="126" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="12" t="s">
         <v>401</v>
       </c>
@@ -7315,7 +7331,7 @@
       <c r="Q126" s="15"/>
       <c r="R126" s="15"/>
     </row>
-    <row r="127" spans="1:18" ht="49.5" customHeight="1">
+    <row r="127" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="12" t="s">
         <v>401</v>
       </c>
@@ -7359,7 +7375,7 @@
       <c r="Q127" s="15"/>
       <c r="R127" s="15"/>
     </row>
-    <row r="128" spans="1:18" ht="49.5" customHeight="1">
+    <row r="128" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="12" t="s">
         <v>401</v>
       </c>
@@ -7407,7 +7423,7 @@
       <c r="Q128" s="15"/>
       <c r="R128" s="15"/>
     </row>
-    <row r="129" spans="1:18" ht="49.5" customHeight="1">
+    <row r="129" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="12" t="s">
         <v>401</v>
       </c>
@@ -7451,7 +7467,7 @@
       <c r="Q129" s="15"/>
       <c r="R129" s="15"/>
     </row>
-    <row r="130" spans="1:18" ht="49.5" customHeight="1">
+    <row r="130" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="12" t="s">
         <v>401</v>
       </c>
@@ -7499,7 +7515,7 @@
       <c r="Q130" s="15"/>
       <c r="R130" s="15"/>
     </row>
-    <row r="131" spans="1:18" ht="49.5" customHeight="1">
+    <row r="131" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="12" t="s">
         <v>401</v>
       </c>
@@ -7543,7 +7559,7 @@
       <c r="Q131" s="15"/>
       <c r="R131" s="15"/>
     </row>
-    <row r="132" spans="1:18" ht="49.5" customHeight="1">
+    <row r="132" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="12" t="s">
         <v>401</v>
       </c>
@@ -7587,7 +7603,7 @@
       <c r="Q132" s="15"/>
       <c r="R132" s="15"/>
     </row>
-    <row r="133" spans="1:18" ht="49.5" customHeight="1">
+    <row r="133" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="12" t="s">
         <v>401</v>
       </c>
@@ -7631,7 +7647,7 @@
       <c r="Q133" s="15"/>
       <c r="R133" s="15"/>
     </row>
-    <row r="134" spans="1:18" ht="49.5" customHeight="1">
+    <row r="134" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="12" t="s">
         <v>401</v>
       </c>
@@ -7679,7 +7695,7 @@
       <c r="Q134" s="15"/>
       <c r="R134" s="15"/>
     </row>
-    <row r="135" spans="1:18" ht="49.5" customHeight="1">
+    <row r="135" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="12" t="s">
         <v>401</v>
       </c>
@@ -7719,7 +7735,7 @@
       <c r="Q135" s="15"/>
       <c r="R135" s="15"/>
     </row>
-    <row r="136" spans="1:18" ht="49.5" customHeight="1">
+    <row r="136" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="12" t="s">
         <v>401</v>
       </c>
@@ -7767,7 +7783,7 @@
       <c r="Q136" s="15"/>
       <c r="R136" s="15"/>
     </row>
-    <row r="137" spans="1:18" ht="49.5" customHeight="1">
+    <row r="137" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="12" t="s">
         <v>401</v>
       </c>
@@ -7811,7 +7827,7 @@
       <c r="Q137" s="15"/>
       <c r="R137" s="15"/>
     </row>
-    <row r="138" spans="1:18" ht="49.5" customHeight="1">
+    <row r="138" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="12" t="s">
         <v>401</v>
       </c>
@@ -7855,7 +7871,7 @@
       <c r="Q138" s="15"/>
       <c r="R138" s="15"/>
     </row>
-    <row r="139" spans="1:18" ht="49.5" customHeight="1">
+    <row r="139" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="12" t="s">
         <v>401</v>
       </c>
@@ -7903,7 +7919,7 @@
       <c r="Q139" s="15"/>
       <c r="R139" s="15"/>
     </row>
-    <row r="140" spans="1:18" ht="49.5" customHeight="1">
+    <row r="140" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="12" t="s">
         <v>401</v>
       </c>
@@ -7951,7 +7967,7 @@
       <c r="Q140" s="15"/>
       <c r="R140" s="15"/>
     </row>
-    <row r="141" spans="1:18" ht="49.5" customHeight="1">
+    <row r="141" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="12" t="s">
         <v>401</v>
       </c>
@@ -7999,7 +8015,7 @@
       <c r="Q141" s="15"/>
       <c r="R141" s="15"/>
     </row>
-    <row r="142" spans="1:18" ht="49.5" customHeight="1">
+    <row r="142" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="12" t="s">
         <v>401</v>
       </c>
@@ -8055,4 +8071,124 @@
     <oddFooter>第 &amp;P 頁</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+      <c r="A1" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="14">
+        <v>2</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="15">
+        <v>2800</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" s="15">
+        <v>10746487</v>
+      </c>
+      <c r="J2" s="15">
+        <v>80</v>
+      </c>
+      <c r="K2" s="15">
+        <v>10748713</v>
+      </c>
+      <c r="L2" s="15">
+        <v>2720</v>
+      </c>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug for kyca
</commit_message>
<xml_diff>
--- a/FrmPIE/0temple/templesforKYCA.xlsx
+++ b/FrmPIE/0temple/templesforKYCA.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\0work\2014\gitpie\FrmPIE\0temple\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14715" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="0105" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="0105" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'0105'!$A$1:$T$142</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'0105'!$1:$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'0105'!$A$1:$T$142</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'0105'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="423">
   <si>
     <t>7YCS12B1008+H01</t>
   </si>
@@ -1256,16 +1251,57 @@
   </si>
   <si>
     <t>20110655-12R1F</t>
+  </si>
+  <si>
+    <t>PO1</t>
+  </si>
+  <si>
+    <t>PO2</t>
+  </si>
+  <si>
+    <t>PO3</t>
+  </si>
+  <si>
+    <t>50501201R2F</t>
+  </si>
+  <si>
+    <t>2-12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K-1-5-16A</t>
+  </si>
+  <si>
+    <t>7YCS12B1008+H02</t>
+  </si>
+  <si>
+    <t>JSTT01</t>
+  </si>
+  <si>
+    <t>PO4</t>
+  </si>
+  <si>
+    <t>50501201R3F</t>
+  </si>
+  <si>
+    <t>K-1-5-17A</t>
+  </si>
+  <si>
+    <t>7YCS12B1008+H03</t>
+  </si>
+  <si>
+    <t>2-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -1280,6 +1316,12 @@
       <sz val="10"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1296,7 +1338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1330,13 +1372,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1406,6 +1461,18 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1466,7 +1533,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1498,10 +1565,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1533,7 +1599,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1709,14 +1774,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="12">
+      <c r="A1" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="14">
+        <v>2</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="15">
+        <v>2800</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" s="15">
+        <v>10746487</v>
+      </c>
+      <c r="J2" s="15">
+        <v>80</v>
+      </c>
+      <c r="K2" s="15">
+        <v>10748713</v>
+      </c>
+      <c r="L2" s="15">
+        <v>2720</v>
+      </c>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" thickBot="1">
+      <c r="A3" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>414</v>
+      </c>
+      <c r="E3" s="14">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="G3" s="23">
+        <v>7839</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J3" s="23">
+        <v>2800</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="L3" s="23">
+        <v>5000</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>412</v>
+      </c>
+      <c r="N3" s="23">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" thickBot="1">
+      <c r="A4" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="E4" s="14">
+        <v>4</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="G4" s="23">
+        <v>5461</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J4" s="23">
+        <v>1500</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="L4" s="23">
+        <v>2000</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>412</v>
+      </c>
+      <c r="N4" s="23">
+        <v>1000</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>418</v>
+      </c>
+      <c r="P4" s="23">
+        <v>961</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="11.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" style="1" bestFit="1" customWidth="1"/>
@@ -1741,7 +2021,7 @@
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" s="2" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>400</v>
       </c>
@@ -1799,7 +2079,7 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" ht="49.5" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>401</v>
       </c>
@@ -1847,7 +2127,7 @@
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
     </row>
-    <row r="3" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" ht="49.5" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>401</v>
       </c>
@@ -1887,7 +2167,7 @@
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
     </row>
-    <row r="4" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" ht="49.5" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>401</v>
       </c>
@@ -1931,7 +2211,7 @@
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" ht="49.5" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>401</v>
       </c>
@@ -1975,7 +2255,7 @@
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="6" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" ht="49.5" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>401</v>
       </c>
@@ -2023,7 +2303,7 @@
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
     </row>
-    <row r="7" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" ht="49.5" customHeight="1">
       <c r="A7" s="12" t="s">
         <v>401</v>
       </c>
@@ -2067,7 +2347,7 @@
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
     </row>
-    <row r="8" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" ht="49.5" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>401</v>
       </c>
@@ -2115,7 +2395,7 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" ht="49.5" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>401</v>
       </c>
@@ -2159,7 +2439,7 @@
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="10" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" ht="49.5" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>401</v>
       </c>
@@ -2203,7 +2483,7 @@
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
     </row>
-    <row r="11" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" ht="49.5" customHeight="1">
       <c r="A11" s="12" t="s">
         <v>401</v>
       </c>
@@ -2251,7 +2531,7 @@
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
     </row>
-    <row r="12" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" ht="49.5" customHeight="1">
       <c r="A12" s="12" t="s">
         <v>401</v>
       </c>
@@ -2299,7 +2579,7 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
     </row>
-    <row r="13" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" ht="49.5" customHeight="1">
       <c r="A13" s="12" t="s">
         <v>401</v>
       </c>
@@ -2339,7 +2619,7 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
     </row>
-    <row r="14" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" ht="49.5" customHeight="1">
       <c r="A14" s="12" t="s">
         <v>401</v>
       </c>
@@ -2379,7 +2659,7 @@
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
     </row>
-    <row r="15" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" ht="49.5" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>401</v>
       </c>
@@ -2419,7 +2699,7 @@
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
     </row>
-    <row r="16" spans="1:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" ht="49.5" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>401</v>
       </c>
@@ -2463,7 +2743,7 @@
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
     </row>
-    <row r="17" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" ht="49.5" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>401</v>
       </c>
@@ -2511,7 +2791,7 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" ht="49.5" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>401</v>
       </c>
@@ -2555,7 +2835,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" ht="49.5" customHeight="1">
       <c r="A19" s="12" t="s">
         <v>401</v>
       </c>
@@ -2599,7 +2879,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" ht="49.5" customHeight="1">
       <c r="A20" s="12" t="s">
         <v>401</v>
       </c>
@@ -2643,7 +2923,7 @@
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" ht="49.5" customHeight="1">
       <c r="A21" s="12" t="s">
         <v>401</v>
       </c>
@@ -2687,7 +2967,7 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" ht="49.5" customHeight="1">
       <c r="A22" s="12" t="s">
         <v>401</v>
       </c>
@@ -2731,7 +3011,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" ht="49.5" customHeight="1">
       <c r="A23" s="12" t="s">
         <v>401</v>
       </c>
@@ -2775,7 +3055,7 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" ht="49.5" customHeight="1">
       <c r="A24" s="12" t="s">
         <v>401</v>
       </c>
@@ -2819,7 +3099,7 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" ht="49.5" customHeight="1">
       <c r="A25" s="12" t="s">
         <v>401</v>
       </c>
@@ -2871,7 +3151,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" ht="49.5" customHeight="1">
       <c r="A26" s="12" t="s">
         <v>401</v>
       </c>
@@ -2911,7 +3191,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" ht="49.5" customHeight="1">
       <c r="A27" s="12" t="s">
         <v>401</v>
       </c>
@@ -2955,7 +3235,7 @@
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
     </row>
-    <row r="28" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:18" ht="49.5" customHeight="1">
       <c r="A28" s="12" t="s">
         <v>401</v>
       </c>
@@ -2995,7 +3275,7 @@
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
     </row>
-    <row r="29" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" ht="49.5" customHeight="1">
       <c r="A29" s="12" t="s">
         <v>401</v>
       </c>
@@ -3043,7 +3323,7 @@
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
     </row>
-    <row r="30" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" ht="49.5" customHeight="1">
       <c r="A30" s="12" t="s">
         <v>401</v>
       </c>
@@ -3091,7 +3371,7 @@
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
     </row>
-    <row r="31" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" ht="49.5" customHeight="1">
       <c r="A31" s="12" t="s">
         <v>401</v>
       </c>
@@ -3135,7 +3415,7 @@
       <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
     </row>
-    <row r="32" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:18" ht="49.5" customHeight="1">
       <c r="A32" s="12" t="s">
         <v>401</v>
       </c>
@@ -3179,7 +3459,7 @@
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
     </row>
-    <row r="33" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:18" ht="49.5" customHeight="1">
       <c r="A33" s="12" t="s">
         <v>401</v>
       </c>
@@ -3223,7 +3503,7 @@
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
     </row>
-    <row r="34" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" ht="49.5" customHeight="1">
       <c r="A34" s="12" t="s">
         <v>401</v>
       </c>
@@ -3267,7 +3547,7 @@
       <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
     </row>
-    <row r="35" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" ht="49.5" customHeight="1">
       <c r="A35" s="12" t="s">
         <v>401</v>
       </c>
@@ -3311,7 +3591,7 @@
       <c r="Q35" s="15"/>
       <c r="R35" s="15"/>
     </row>
-    <row r="36" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" ht="49.5" customHeight="1">
       <c r="A36" s="12" t="s">
         <v>401</v>
       </c>
@@ -3359,7 +3639,7 @@
       <c r="Q36" s="15"/>
       <c r="R36" s="15"/>
     </row>
-    <row r="37" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" ht="49.5" customHeight="1">
       <c r="A37" s="12" t="s">
         <v>401</v>
       </c>
@@ -3407,7 +3687,7 @@
       <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
     </row>
-    <row r="38" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" ht="49.5" customHeight="1">
       <c r="A38" s="12" t="s">
         <v>401</v>
       </c>
@@ -3455,7 +3735,7 @@
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
     </row>
-    <row r="39" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" ht="49.5" customHeight="1">
       <c r="A39" s="12" t="s">
         <v>401</v>
       </c>
@@ -3503,7 +3783,7 @@
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
     </row>
-    <row r="40" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:18" ht="49.5" customHeight="1">
       <c r="A40" s="12" t="s">
         <v>401</v>
       </c>
@@ -3547,7 +3827,7 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
     </row>
-    <row r="41" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:18" ht="49.5" customHeight="1">
       <c r="A41" s="12" t="s">
         <v>401</v>
       </c>
@@ -3595,7 +3875,7 @@
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
     </row>
-    <row r="42" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" ht="49.5" customHeight="1">
       <c r="A42" s="12" t="s">
         <v>401</v>
       </c>
@@ -3639,7 +3919,7 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
     </row>
-    <row r="43" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" ht="49.5" customHeight="1">
       <c r="A43" s="12" t="s">
         <v>401</v>
       </c>
@@ -3687,7 +3967,7 @@
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
     </row>
-    <row r="44" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" ht="49.5" customHeight="1">
       <c r="A44" s="12" t="s">
         <v>401</v>
       </c>
@@ -3727,7 +4007,7 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
     </row>
-    <row r="45" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" ht="49.5" customHeight="1">
       <c r="A45" s="12" t="s">
         <v>401</v>
       </c>
@@ -3771,7 +4051,7 @@
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
     </row>
-    <row r="46" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:18" ht="49.5" customHeight="1">
       <c r="A46" s="12" t="s">
         <v>401</v>
       </c>
@@ -3819,7 +4099,7 @@
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
     </row>
-    <row r="47" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" ht="49.5" customHeight="1">
       <c r="A47" s="12" t="s">
         <v>401</v>
       </c>
@@ -3859,7 +4139,7 @@
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
     </row>
-    <row r="48" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:18" ht="49.5" customHeight="1">
       <c r="A48" s="12" t="s">
         <v>401</v>
       </c>
@@ -3899,7 +4179,7 @@
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
     </row>
-    <row r="49" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" ht="49.5" customHeight="1">
       <c r="A49" s="12" t="s">
         <v>401</v>
       </c>
@@ -3943,7 +4223,7 @@
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
     </row>
-    <row r="50" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" ht="49.5" customHeight="1">
       <c r="A50" s="12" t="s">
         <v>401</v>
       </c>
@@ -3987,7 +4267,7 @@
       <c r="Q50" s="15"/>
       <c r="R50" s="15"/>
     </row>
-    <row r="51" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:18" ht="49.5" customHeight="1">
       <c r="A51" s="12" t="s">
         <v>401</v>
       </c>
@@ -4031,7 +4311,7 @@
       <c r="Q51" s="15"/>
       <c r="R51" s="15"/>
     </row>
-    <row r="52" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:18" ht="49.5" customHeight="1">
       <c r="A52" s="12" t="s">
         <v>401</v>
       </c>
@@ -4075,7 +4355,7 @@
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
     </row>
-    <row r="53" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:18" ht="49.5" customHeight="1">
       <c r="A53" s="12" t="s">
         <v>401</v>
       </c>
@@ -4119,7 +4399,7 @@
       <c r="Q53" s="15"/>
       <c r="R53" s="15"/>
     </row>
-    <row r="54" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:18" ht="49.5" customHeight="1">
       <c r="A54" s="12" t="s">
         <v>401</v>
       </c>
@@ -4167,7 +4447,7 @@
       <c r="Q54" s="15"/>
       <c r="R54" s="15"/>
     </row>
-    <row r="55" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:18" ht="49.5" customHeight="1">
       <c r="A55" s="12" t="s">
         <v>401</v>
       </c>
@@ -4219,7 +4499,7 @@
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
     </row>
-    <row r="56" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:18" ht="49.5" customHeight="1">
       <c r="A56" s="12" t="s">
         <v>401</v>
       </c>
@@ -4259,7 +4539,7 @@
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
     </row>
-    <row r="57" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:18" ht="49.5" customHeight="1">
       <c r="A57" s="12" t="s">
         <v>401</v>
       </c>
@@ -4307,7 +4587,7 @@
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
     </row>
-    <row r="58" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:18" ht="49.5" customHeight="1">
       <c r="A58" s="12" t="s">
         <v>401</v>
       </c>
@@ -4355,7 +4635,7 @@
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
     </row>
-    <row r="59" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:18" ht="49.5" customHeight="1">
       <c r="A59" s="12" t="s">
         <v>401</v>
       </c>
@@ -4399,7 +4679,7 @@
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
     </row>
-    <row r="60" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:18" ht="49.5" customHeight="1">
       <c r="A60" s="12" t="s">
         <v>401</v>
       </c>
@@ -4439,7 +4719,7 @@
       <c r="Q60" s="15"/>
       <c r="R60" s="15"/>
     </row>
-    <row r="61" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:18" ht="49.5" customHeight="1">
       <c r="A61" s="12" t="s">
         <v>401</v>
       </c>
@@ -4479,7 +4759,7 @@
       <c r="Q61" s="15"/>
       <c r="R61" s="15"/>
     </row>
-    <row r="62" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:18" ht="49.5" customHeight="1">
       <c r="A62" s="12" t="s">
         <v>401</v>
       </c>
@@ -4535,7 +4815,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:18" ht="49.5" customHeight="1">
       <c r="A63" s="12" t="s">
         <v>401</v>
       </c>
@@ -4575,7 +4855,7 @@
       <c r="Q63" s="15"/>
       <c r="R63" s="15"/>
     </row>
-    <row r="64" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:18" ht="49.5" customHeight="1">
       <c r="A64" s="12" t="s">
         <v>401</v>
       </c>
@@ -4619,7 +4899,7 @@
       <c r="Q64" s="15"/>
       <c r="R64" s="15"/>
     </row>
-    <row r="65" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:18" ht="49.5" customHeight="1">
       <c r="A65" s="12" t="s">
         <v>401</v>
       </c>
@@ -4663,7 +4943,7 @@
       <c r="Q65" s="15"/>
       <c r="R65" s="15"/>
     </row>
-    <row r="66" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:18" ht="49.5" customHeight="1">
       <c r="A66" s="12" t="s">
         <v>401</v>
       </c>
@@ -4707,7 +4987,7 @@
       <c r="Q66" s="15"/>
       <c r="R66" s="15"/>
     </row>
-    <row r="67" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:18" ht="49.5" customHeight="1">
       <c r="A67" s="12" t="s">
         <v>401</v>
       </c>
@@ -4747,7 +5027,7 @@
       <c r="Q67" s="15"/>
       <c r="R67" s="15"/>
     </row>
-    <row r="68" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:18" ht="49.5" customHeight="1">
       <c r="A68" s="12" t="s">
         <v>401</v>
       </c>
@@ -4791,7 +5071,7 @@
       <c r="Q68" s="15"/>
       <c r="R68" s="15"/>
     </row>
-    <row r="69" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:18" ht="49.5" customHeight="1">
       <c r="A69" s="12" t="s">
         <v>401</v>
       </c>
@@ -4835,7 +5115,7 @@
       <c r="Q69" s="15"/>
       <c r="R69" s="15"/>
     </row>
-    <row r="70" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:18" ht="49.5" customHeight="1">
       <c r="A70" s="12" t="s">
         <v>401</v>
       </c>
@@ -4883,7 +5163,7 @@
       <c r="Q70" s="15"/>
       <c r="R70" s="15"/>
     </row>
-    <row r="71" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:18" ht="49.5" customHeight="1">
       <c r="A71" s="12" t="s">
         <v>401</v>
       </c>
@@ -4923,7 +5203,7 @@
       <c r="Q71" s="15"/>
       <c r="R71" s="15"/>
     </row>
-    <row r="72" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:18" ht="49.5" customHeight="1">
       <c r="A72" s="12" t="s">
         <v>401</v>
       </c>
@@ -4967,7 +5247,7 @@
       <c r="Q72" s="15"/>
       <c r="R72" s="15"/>
     </row>
-    <row r="73" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:18" ht="49.5" customHeight="1">
       <c r="A73" s="12" t="s">
         <v>401</v>
       </c>
@@ -5015,7 +5295,7 @@
       <c r="Q73" s="15"/>
       <c r="R73" s="15"/>
     </row>
-    <row r="74" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:18" ht="49.5" customHeight="1">
       <c r="A74" s="12" t="s">
         <v>401</v>
       </c>
@@ -5059,7 +5339,7 @@
       <c r="Q74" s="15"/>
       <c r="R74" s="15"/>
     </row>
-    <row r="75" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:18" ht="49.5" customHeight="1">
       <c r="A75" s="12" t="s">
         <v>401</v>
       </c>
@@ -5103,7 +5383,7 @@
       <c r="Q75" s="15"/>
       <c r="R75" s="15"/>
     </row>
-    <row r="76" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:18" ht="49.5" customHeight="1">
       <c r="A76" s="12" t="s">
         <v>401</v>
       </c>
@@ -5147,7 +5427,7 @@
       <c r="Q76" s="15"/>
       <c r="R76" s="15"/>
     </row>
-    <row r="77" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:18" ht="49.5" customHeight="1">
       <c r="A77" s="12" t="s">
         <v>401</v>
       </c>
@@ -5191,7 +5471,7 @@
       <c r="Q77" s="15"/>
       <c r="R77" s="15"/>
     </row>
-    <row r="78" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:18" ht="49.5" customHeight="1">
       <c r="A78" s="12" t="s">
         <v>401</v>
       </c>
@@ -5235,7 +5515,7 @@
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
     </row>
-    <row r="79" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:18" ht="49.5" customHeight="1">
       <c r="A79" s="12" t="s">
         <v>401</v>
       </c>
@@ -5283,7 +5563,7 @@
       <c r="Q79" s="15"/>
       <c r="R79" s="15"/>
     </row>
-    <row r="80" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:18" ht="49.5" customHeight="1">
       <c r="A80" s="12" t="s">
         <v>401</v>
       </c>
@@ -5323,7 +5603,7 @@
       <c r="Q80" s="15"/>
       <c r="R80" s="15"/>
     </row>
-    <row r="81" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:18" ht="49.5" customHeight="1">
       <c r="A81" s="12" t="s">
         <v>401</v>
       </c>
@@ -5367,7 +5647,7 @@
       <c r="Q81" s="15"/>
       <c r="R81" s="15"/>
     </row>
-    <row r="82" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:18" ht="49.5" customHeight="1">
       <c r="A82" s="12" t="s">
         <v>401</v>
       </c>
@@ -5415,7 +5695,7 @@
       <c r="Q82" s="15"/>
       <c r="R82" s="15"/>
     </row>
-    <row r="83" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:18" ht="49.5" customHeight="1">
       <c r="A83" s="12" t="s">
         <v>401</v>
       </c>
@@ -5459,7 +5739,7 @@
       <c r="Q83" s="15"/>
       <c r="R83" s="15"/>
     </row>
-    <row r="84" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:18" ht="49.5" customHeight="1">
       <c r="A84" s="12" t="s">
         <v>401</v>
       </c>
@@ -5503,7 +5783,7 @@
       <c r="Q84" s="15"/>
       <c r="R84" s="15"/>
     </row>
-    <row r="85" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:18" ht="49.5" customHeight="1">
       <c r="A85" s="12" t="s">
         <v>401</v>
       </c>
@@ -5543,7 +5823,7 @@
       <c r="Q85" s="15"/>
       <c r="R85" s="15"/>
     </row>
-    <row r="86" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:18" ht="49.5" customHeight="1">
       <c r="A86" s="12" t="s">
         <v>401</v>
       </c>
@@ -5591,7 +5871,7 @@
       <c r="Q86" s="15"/>
       <c r="R86" s="15"/>
     </row>
-    <row r="87" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:18" ht="49.5" customHeight="1">
       <c r="A87" s="12" t="s">
         <v>401</v>
       </c>
@@ -5631,7 +5911,7 @@
       <c r="Q87" s="15"/>
       <c r="R87" s="15"/>
     </row>
-    <row r="88" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:18" ht="49.5" customHeight="1">
       <c r="A88" s="12" t="s">
         <v>401</v>
       </c>
@@ -5675,7 +5955,7 @@
       <c r="Q88" s="15"/>
       <c r="R88" s="15"/>
     </row>
-    <row r="89" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:18" ht="49.5" customHeight="1">
       <c r="A89" s="12" t="s">
         <v>401</v>
       </c>
@@ -5719,7 +5999,7 @@
       <c r="Q89" s="15"/>
       <c r="R89" s="15"/>
     </row>
-    <row r="90" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:18" ht="49.5" customHeight="1">
       <c r="A90" s="12" t="s">
         <v>401</v>
       </c>
@@ -5763,7 +6043,7 @@
       <c r="Q90" s="15"/>
       <c r="R90" s="15"/>
     </row>
-    <row r="91" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:18" ht="49.5" customHeight="1">
       <c r="A91" s="12" t="s">
         <v>401</v>
       </c>
@@ -5803,7 +6083,7 @@
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
     </row>
-    <row r="92" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:18" ht="49.5" customHeight="1">
       <c r="A92" s="12" t="s">
         <v>401</v>
       </c>
@@ -5851,7 +6131,7 @@
       <c r="Q92" s="15"/>
       <c r="R92" s="15"/>
     </row>
-    <row r="93" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:18" ht="49.5" customHeight="1">
       <c r="A93" s="12" t="s">
         <v>401</v>
       </c>
@@ -5895,7 +6175,7 @@
       <c r="Q93" s="15"/>
       <c r="R93" s="15"/>
     </row>
-    <row r="94" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:18" ht="49.5" customHeight="1">
       <c r="A94" s="12" t="s">
         <v>401</v>
       </c>
@@ -5935,7 +6215,7 @@
       <c r="Q94" s="15"/>
       <c r="R94" s="15"/>
     </row>
-    <row r="95" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:18" ht="49.5" customHeight="1">
       <c r="A95" s="12" t="s">
         <v>401</v>
       </c>
@@ -5979,7 +6259,7 @@
       <c r="Q95" s="15"/>
       <c r="R95" s="15"/>
     </row>
-    <row r="96" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:18" ht="49.5" customHeight="1">
       <c r="A96" s="12" t="s">
         <v>401</v>
       </c>
@@ -6023,7 +6303,7 @@
       <c r="Q96" s="15"/>
       <c r="R96" s="15"/>
     </row>
-    <row r="97" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:18" ht="49.5" customHeight="1">
       <c r="A97" s="12" t="s">
         <v>401</v>
       </c>
@@ -6067,7 +6347,7 @@
       <c r="Q97" s="15"/>
       <c r="R97" s="15"/>
     </row>
-    <row r="98" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:18" ht="49.5" customHeight="1">
       <c r="A98" s="12" t="s">
         <v>401</v>
       </c>
@@ -6115,7 +6395,7 @@
       <c r="Q98" s="15"/>
       <c r="R98" s="15"/>
     </row>
-    <row r="99" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:18" ht="49.5" customHeight="1">
       <c r="A99" s="12" t="s">
         <v>401</v>
       </c>
@@ -6155,7 +6435,7 @@
       <c r="Q99" s="15"/>
       <c r="R99" s="15"/>
     </row>
-    <row r="100" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:18" ht="49.5" customHeight="1">
       <c r="A100" s="12" t="s">
         <v>401</v>
       </c>
@@ -6199,7 +6479,7 @@
       <c r="Q100" s="15"/>
       <c r="R100" s="15"/>
     </row>
-    <row r="101" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:18" ht="49.5" customHeight="1">
       <c r="A101" s="12" t="s">
         <v>401</v>
       </c>
@@ -6239,7 +6519,7 @@
       <c r="Q101" s="15"/>
       <c r="R101" s="15"/>
     </row>
-    <row r="102" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:18" ht="49.5" customHeight="1">
       <c r="A102" s="12" t="s">
         <v>401</v>
       </c>
@@ -6279,7 +6559,7 @@
       <c r="Q102" s="15"/>
       <c r="R102" s="15"/>
     </row>
-    <row r="103" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:18" ht="49.5" customHeight="1">
       <c r="A103" s="12" t="s">
         <v>401</v>
       </c>
@@ -6319,7 +6599,7 @@
       <c r="Q103" s="15"/>
       <c r="R103" s="15"/>
     </row>
-    <row r="104" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:18" ht="49.5" customHeight="1">
       <c r="A104" s="12" t="s">
         <v>401</v>
       </c>
@@ -6359,7 +6639,7 @@
       <c r="Q104" s="15"/>
       <c r="R104" s="15"/>
     </row>
-    <row r="105" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:18" ht="49.5" customHeight="1">
       <c r="A105" s="12" t="s">
         <v>401</v>
       </c>
@@ -6399,7 +6679,7 @@
       <c r="Q105" s="15"/>
       <c r="R105" s="15"/>
     </row>
-    <row r="106" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:18" ht="49.5" customHeight="1">
       <c r="A106" s="12" t="s">
         <v>401</v>
       </c>
@@ -6439,7 +6719,7 @@
       <c r="Q106" s="15"/>
       <c r="R106" s="15"/>
     </row>
-    <row r="107" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:18" ht="49.5" customHeight="1">
       <c r="A107" s="12" t="s">
         <v>401</v>
       </c>
@@ -6483,7 +6763,7 @@
       <c r="Q107" s="15"/>
       <c r="R107" s="15"/>
     </row>
-    <row r="108" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:18" ht="49.5" customHeight="1">
       <c r="A108" s="12" t="s">
         <v>401</v>
       </c>
@@ -6523,7 +6803,7 @@
       <c r="Q108" s="15"/>
       <c r="R108" s="15"/>
     </row>
-    <row r="109" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:18" ht="49.5" customHeight="1">
       <c r="A109" s="12" t="s">
         <v>401</v>
       </c>
@@ -6563,7 +6843,7 @@
       <c r="Q109" s="15"/>
       <c r="R109" s="15"/>
     </row>
-    <row r="110" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:18" ht="49.5" customHeight="1">
       <c r="A110" s="12" t="s">
         <v>401</v>
       </c>
@@ -6607,7 +6887,7 @@
       <c r="Q110" s="15"/>
       <c r="R110" s="15"/>
     </row>
-    <row r="111" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:18" ht="49.5" customHeight="1">
       <c r="A111" s="12" t="s">
         <v>401</v>
       </c>
@@ -6655,7 +6935,7 @@
       <c r="Q111" s="15"/>
       <c r="R111" s="15"/>
     </row>
-    <row r="112" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:18" ht="49.5" customHeight="1">
       <c r="A112" s="12" t="s">
         <v>401</v>
       </c>
@@ -6699,7 +6979,7 @@
       <c r="Q112" s="15"/>
       <c r="R112" s="15"/>
     </row>
-    <row r="113" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:18" ht="49.5" customHeight="1">
       <c r="A113" s="12" t="s">
         <v>401</v>
       </c>
@@ -6743,7 +7023,7 @@
       <c r="Q113" s="15"/>
       <c r="R113" s="15"/>
     </row>
-    <row r="114" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:18" ht="49.5" customHeight="1">
       <c r="A114" s="12" t="s">
         <v>401</v>
       </c>
@@ -6787,7 +7067,7 @@
       <c r="Q114" s="15"/>
       <c r="R114" s="15"/>
     </row>
-    <row r="115" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:18" ht="49.5" customHeight="1">
       <c r="A115" s="12" t="s">
         <v>401</v>
       </c>
@@ -6831,7 +7111,7 @@
       <c r="Q115" s="15"/>
       <c r="R115" s="15"/>
     </row>
-    <row r="116" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:18" ht="49.5" customHeight="1">
       <c r="A116" s="12" t="s">
         <v>401</v>
       </c>
@@ -6879,7 +7159,7 @@
       <c r="Q116" s="15"/>
       <c r="R116" s="15"/>
     </row>
-    <row r="117" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:18" ht="49.5" customHeight="1">
       <c r="A117" s="12" t="s">
         <v>401</v>
       </c>
@@ -6919,7 +7199,7 @@
       <c r="Q117" s="15"/>
       <c r="R117" s="15"/>
     </row>
-    <row r="118" spans="1:18" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" ht="49.5" customHeight="1" thickBot="1">
       <c r="A118" s="12" t="s">
         <v>401</v>
       </c>
@@ -6963,7 +7243,7 @@
       <c r="Q118" s="15"/>
       <c r="R118" s="15"/>
     </row>
-    <row r="119" spans="1:18" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" ht="49.5" customHeight="1" thickBot="1">
       <c r="A119" s="12" t="s">
         <v>401</v>
       </c>
@@ -7011,7 +7291,7 @@
       <c r="Q119" s="15"/>
       <c r="R119" s="15"/>
     </row>
-    <row r="120" spans="1:18" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" ht="49.5" customHeight="1" thickBot="1">
       <c r="A120" s="12" t="s">
         <v>401</v>
       </c>
@@ -7059,7 +7339,7 @@
       <c r="Q120" s="15"/>
       <c r="R120" s="15"/>
     </row>
-    <row r="121" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:18" ht="49.5" customHeight="1">
       <c r="A121" s="12" t="s">
         <v>401</v>
       </c>
@@ -7103,7 +7383,7 @@
       <c r="Q121" s="15"/>
       <c r="R121" s="15"/>
     </row>
-    <row r="122" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:18" ht="49.5" customHeight="1">
       <c r="A122" s="12" t="s">
         <v>401</v>
       </c>
@@ -7147,7 +7427,7 @@
       <c r="Q122" s="15"/>
       <c r="R122" s="15"/>
     </row>
-    <row r="123" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:18" ht="49.5" customHeight="1">
       <c r="A123" s="12" t="s">
         <v>401</v>
       </c>
@@ -7191,7 +7471,7 @@
       <c r="Q123" s="15"/>
       <c r="R123" s="15"/>
     </row>
-    <row r="124" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:18" ht="49.5" customHeight="1">
       <c r="A124" s="12" t="s">
         <v>401</v>
       </c>
@@ -7235,7 +7515,7 @@
       <c r="Q124" s="15"/>
       <c r="R124" s="15"/>
     </row>
-    <row r="125" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:18" ht="49.5" customHeight="1">
       <c r="A125" s="12" t="s">
         <v>401</v>
       </c>
@@ -7283,7 +7563,7 @@
       <c r="Q125" s="15"/>
       <c r="R125" s="15"/>
     </row>
-    <row r="126" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:18" ht="49.5" customHeight="1">
       <c r="A126" s="12" t="s">
         <v>401</v>
       </c>
@@ -7331,7 +7611,7 @@
       <c r="Q126" s="15"/>
       <c r="R126" s="15"/>
     </row>
-    <row r="127" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:18" ht="49.5" customHeight="1">
       <c r="A127" s="12" t="s">
         <v>401</v>
       </c>
@@ -7375,7 +7655,7 @@
       <c r="Q127" s="15"/>
       <c r="R127" s="15"/>
     </row>
-    <row r="128" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:18" ht="49.5" customHeight="1">
       <c r="A128" s="12" t="s">
         <v>401</v>
       </c>
@@ -7423,7 +7703,7 @@
       <c r="Q128" s="15"/>
       <c r="R128" s="15"/>
     </row>
-    <row r="129" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:18" ht="49.5" customHeight="1">
       <c r="A129" s="12" t="s">
         <v>401</v>
       </c>
@@ -7467,7 +7747,7 @@
       <c r="Q129" s="15"/>
       <c r="R129" s="15"/>
     </row>
-    <row r="130" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:18" ht="49.5" customHeight="1">
       <c r="A130" s="12" t="s">
         <v>401</v>
       </c>
@@ -7515,7 +7795,7 @@
       <c r="Q130" s="15"/>
       <c r="R130" s="15"/>
     </row>
-    <row r="131" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:18" ht="49.5" customHeight="1">
       <c r="A131" s="12" t="s">
         <v>401</v>
       </c>
@@ -7559,7 +7839,7 @@
       <c r="Q131" s="15"/>
       <c r="R131" s="15"/>
     </row>
-    <row r="132" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:18" ht="49.5" customHeight="1">
       <c r="A132" s="12" t="s">
         <v>401</v>
       </c>
@@ -7603,7 +7883,7 @@
       <c r="Q132" s="15"/>
       <c r="R132" s="15"/>
     </row>
-    <row r="133" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:18" ht="49.5" customHeight="1">
       <c r="A133" s="12" t="s">
         <v>401</v>
       </c>
@@ -7647,7 +7927,7 @@
       <c r="Q133" s="15"/>
       <c r="R133" s="15"/>
     </row>
-    <row r="134" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:18" ht="49.5" customHeight="1">
       <c r="A134" s="12" t="s">
         <v>401</v>
       </c>
@@ -7695,7 +7975,7 @@
       <c r="Q134" s="15"/>
       <c r="R134" s="15"/>
     </row>
-    <row r="135" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:18" ht="49.5" customHeight="1">
       <c r="A135" s="12" t="s">
         <v>401</v>
       </c>
@@ -7735,7 +8015,7 @@
       <c r="Q135" s="15"/>
       <c r="R135" s="15"/>
     </row>
-    <row r="136" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:18" ht="49.5" customHeight="1">
       <c r="A136" s="12" t="s">
         <v>401</v>
       </c>
@@ -7783,7 +8063,7 @@
       <c r="Q136" s="15"/>
       <c r="R136" s="15"/>
     </row>
-    <row r="137" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:18" ht="49.5" customHeight="1">
       <c r="A137" s="12" t="s">
         <v>401</v>
       </c>
@@ -7827,7 +8107,7 @@
       <c r="Q137" s="15"/>
       <c r="R137" s="15"/>
     </row>
-    <row r="138" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:18" ht="49.5" customHeight="1">
       <c r="A138" s="12" t="s">
         <v>401</v>
       </c>
@@ -7871,7 +8151,7 @@
       <c r="Q138" s="15"/>
       <c r="R138" s="15"/>
     </row>
-    <row r="139" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:18" ht="49.5" customHeight="1">
       <c r="A139" s="12" t="s">
         <v>401</v>
       </c>
@@ -7919,7 +8199,7 @@
       <c r="Q139" s="15"/>
       <c r="R139" s="15"/>
     </row>
-    <row r="140" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:18" ht="49.5" customHeight="1">
       <c r="A140" s="12" t="s">
         <v>401</v>
       </c>
@@ -7967,7 +8247,7 @@
       <c r="Q140" s="15"/>
       <c r="R140" s="15"/>
     </row>
-    <row r="141" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:18" ht="49.5" customHeight="1">
       <c r="A141" s="12" t="s">
         <v>401</v>
       </c>
@@ -8015,7 +8295,7 @@
       <c r="Q141" s="15"/>
       <c r="R141" s="15"/>
     </row>
-    <row r="142" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:18" ht="49.5" customHeight="1">
       <c r="A142" s="12" t="s">
         <v>401</v>
       </c>
@@ -8071,124 +8351,4 @@
     <oddFooter>第 &amp;P 頁</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.15">
-      <c r="A1" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>395</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>396</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>398</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-    </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="12" t="s">
-        <v>401</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="E2" s="14">
-        <v>2</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="G2" s="15">
-        <v>2800</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="I2" s="15">
-        <v>10746487</v>
-      </c>
-      <c r="J2" s="15">
-        <v>80</v>
-      </c>
-      <c r="K2" s="15">
-        <v>10748713</v>
-      </c>
-      <c r="L2" s="15">
-        <v>2720</v>
-      </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug for kyca 2
</commit_message>
<xml_diff>
--- a/FrmPIE/0temple/templesforKYCA.xlsx
+++ b/FrmPIE/0temple/templesforKYCA.xlsx
@@ -8,18 +8,19 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="0105" sheetId="1" r:id="rId2"/>
+    <sheet name="test" sheetId="3" r:id="rId2"/>
+    <sheet name="0105" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'0105'!$A$1:$T$142</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'0105'!$1:$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'0105'!$A$1:$T$142</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'0105'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="439">
   <si>
     <t>7YCS12B1008+H01</t>
   </si>
@@ -1256,41 +1257,108 @@
     <t>PO1</t>
   </si>
   <si>
+    <t>50501201R2F</t>
+  </si>
+  <si>
+    <t>K-1-5-16A</t>
+  </si>
+  <si>
+    <t>7YCS12B1008+H02</t>
+  </si>
+  <si>
+    <t>JSTT01</t>
+  </si>
+  <si>
+    <t>50501201R3F</t>
+  </si>
+  <si>
+    <t>K-1-5-17A</t>
+  </si>
+  <si>
+    <t>7YCS12B1008+H03</t>
+  </si>
+  <si>
+    <t>1-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>PO2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PO3</t>
-  </si>
-  <si>
-    <t>50501201R2F</t>
-  </si>
-  <si>
-    <t>2-12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>K-1-5-16A</t>
-  </si>
-  <si>
-    <t>7YCS12B1008+H02</t>
-  </si>
-  <si>
-    <t>JSTT01</t>
+    <t>A3-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B3-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PO4</t>
-  </si>
-  <si>
-    <t>50501201R3F</t>
-  </si>
-  <si>
-    <t>K-1-5-17A</t>
-  </si>
-  <si>
-    <t>7YCS12B1008+H03</t>
-  </si>
-  <si>
-    <t>2-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L5-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PO5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1338,7 +1406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1372,26 +1440,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1466,12 +1521,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1775,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1841,144 +1890,831 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="49.5" customHeight="1">
+    <row r="2" spans="1:20" ht="15" thickBot="1">
       <c r="A2" s="12" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>0</v>
+        <v>413</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>205</v>
+      <c r="D2" s="9" t="s">
+        <v>418</v>
       </c>
       <c r="E2" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="G2" s="15">
-        <v>2800</v>
+        <v>411</v>
+      </c>
+      <c r="G2" s="23">
+        <v>1000</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="I2" s="15">
-        <v>10746487</v>
-      </c>
-      <c r="J2" s="15">
-        <v>80</v>
-      </c>
-      <c r="K2" s="15">
-        <v>10748713</v>
-      </c>
-      <c r="L2" s="15">
-        <v>2720</v>
-      </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
+      <c r="I2" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J2" s="23">
+        <v>1000</v>
+      </c>
+      <c r="K2" s="24"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:20" ht="15" thickBot="1">
       <c r="A3" s="12" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="E3" s="14">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="G3" s="23">
+        <v>1000</v>
+      </c>
+      <c r="H3" s="15" t="s">
         <v>414</v>
-      </c>
-      <c r="E3" s="14">
-        <v>3</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="G3" s="23">
-        <v>7839</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>173</v>
       </c>
       <c r="I3" s="24" t="s">
         <v>410</v>
       </c>
       <c r="J3" s="23">
-        <v>2800</v>
+        <v>500</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="L3" s="23">
-        <v>5000</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="N3" s="23">
-        <v>39</v>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="M3" s="24"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="23"/>
     </row>
     <row r="4" spans="1:20" ht="15" thickBot="1">
       <c r="A4" s="12" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>422</v>
+      <c r="D4" s="9" t="s">
+        <v>423</v>
       </c>
       <c r="E4" s="14">
         <v>4</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G4" s="23">
-        <v>5461</v>
+        <v>1000</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I4" s="24" t="s">
         <v>410</v>
       </c>
       <c r="J4" s="23">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="K4" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L4" s="23">
+        <v>900</v>
+      </c>
+      <c r="M4" s="24"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="23"/>
+    </row>
+    <row r="5" spans="1:20" ht="15" thickBot="1">
+      <c r="A5" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="E5" s="14">
+        <v>4</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="G5" s="23">
+        <v>1000</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J5" s="23">
+        <v>900</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L5" s="23">
+        <v>100</v>
+      </c>
+      <c r="M5" s="24"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="23"/>
+    </row>
+    <row r="6" spans="1:20" ht="15" thickBot="1">
+      <c r="A6" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="E6" s="14">
+        <v>3</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>411</v>
       </c>
-      <c r="L4" s="23">
-        <v>2000</v>
-      </c>
-      <c r="M4" s="24" t="s">
+      <c r="G6" s="23">
+        <v>1000</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J6" s="23">
+        <v>500</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L6" s="23">
+        <v>400</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N6" s="23">
+        <v>100</v>
+      </c>
+      <c r="O6" s="24"/>
+    </row>
+    <row r="7" spans="1:20" ht="15" thickBot="1">
+      <c r="A7" s="12" t="s">
         <v>412</v>
       </c>
-      <c r="N4" s="23">
+      <c r="B7" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E7" s="14">
+        <v>3</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G7" s="23">
         <v>1000</v>
       </c>
-      <c r="O4" s="24" t="s">
-        <v>418</v>
-      </c>
-      <c r="P4" s="23">
-        <v>961</v>
+      <c r="H7" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J7" s="23">
+        <v>100</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L7" s="23">
+        <v>400</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N7" s="23">
+        <v>500</v>
+      </c>
+      <c r="O7" s="24"/>
+    </row>
+    <row r="8" spans="1:20" ht="15" thickBot="1">
+      <c r="A8" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="E8" s="14">
+        <v>3</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G8" s="23">
+        <v>1000</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J8" s="23">
+        <v>600</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L8" s="23">
+        <v>100</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N8" s="23">
+        <v>300</v>
+      </c>
+      <c r="O8" s="24"/>
+    </row>
+    <row r="9" spans="1:20" ht="15" thickBot="1">
+      <c r="A9" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="E9" s="14">
+        <v>3</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G9" s="23">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J9" s="23">
+        <v>500</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L9" s="23">
+        <v>100</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N9" s="23">
+        <v>100</v>
+      </c>
+      <c r="O9" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P9" s="23">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15" thickBot="1">
+      <c r="A10" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="E10" s="14">
+        <v>3</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G10" s="23">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J10" s="23">
+        <v>300</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L10" s="23">
+        <v>100</v>
+      </c>
+      <c r="M10" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N10" s="23">
+        <v>100</v>
+      </c>
+      <c r="O10" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P10" s="23">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="15" thickBot="1">
+      <c r="A11" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E11" s="14">
+        <v>3</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G11" s="23">
+        <v>1000</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J11" s="23">
+        <v>100</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L11" s="23">
+        <v>300</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N11" s="23">
+        <v>500</v>
+      </c>
+      <c r="O11" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P11" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15" thickBot="1">
+      <c r="A12" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="E12" s="14">
+        <v>3</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G12" s="23">
+        <v>1000</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J12" s="23">
+        <v>100</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L12" s="23">
+        <v>500</v>
+      </c>
+      <c r="M12" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N12" s="23">
+        <v>300</v>
+      </c>
+      <c r="O12" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P12" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15" thickBot="1">
+      <c r="A13" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="E13" s="14">
+        <v>3</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G13" s="23">
+        <v>1000</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J13" s="23">
+        <v>100</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L13" s="23">
+        <v>100</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N13" s="23">
+        <v>100</v>
+      </c>
+      <c r="O13" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P13" s="23">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15" thickBot="1">
+      <c r="A14" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="E14" s="14">
+        <v>3</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G14" s="23">
+        <v>1001</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J14" s="23">
+        <v>100</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L14" s="23">
+        <v>100</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N14" s="23">
+        <v>100</v>
+      </c>
+      <c r="O14" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P14" s="23">
+        <v>700</v>
+      </c>
+      <c r="Q14" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="R14" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="15" thickBot="1">
+      <c r="A15" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="E15" s="14">
+        <v>3</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G15" s="23">
+        <v>1001</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J15" s="23">
+        <v>1</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L15" s="23">
+        <v>100</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N15" s="23">
+        <v>100</v>
+      </c>
+      <c r="O15" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P15" s="23">
+        <v>700</v>
+      </c>
+      <c r="Q15" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="R15" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="15" thickBot="1">
+      <c r="A16" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="E16" s="14">
+        <v>3</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G16" s="23">
+        <v>1001</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J16" s="23">
+        <v>1</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L16" s="23">
+        <v>500</v>
+      </c>
+      <c r="M16" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N16" s="23">
+        <v>100</v>
+      </c>
+      <c r="O16" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P16" s="23">
+        <v>300</v>
+      </c>
+      <c r="Q16" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="R16" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15" thickBot="1">
+      <c r="A17" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="E17" s="14">
+        <v>3</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G17" s="23">
+        <v>1001</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J17" s="23">
+        <v>1</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L17" s="23">
+        <v>100</v>
+      </c>
+      <c r="M17" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N17" s="23">
+        <v>100</v>
+      </c>
+      <c r="O17" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P17" s="23">
+        <v>300</v>
+      </c>
+      <c r="Q17" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="R17" s="23">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15" thickBot="1">
+      <c r="A18" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E18" s="14">
+        <v>3</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G18" s="23">
+        <v>1001</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J18" s="23">
+        <v>1</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L18" s="23">
+        <v>100</v>
+      </c>
+      <c r="M18" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N18" s="23">
+        <v>100</v>
+      </c>
+      <c r="O18" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P18" s="23">
+        <v>500</v>
+      </c>
+      <c r="Q18" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="R18" s="23">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1989,6 +2725,248 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="12">
+      <c r="A1" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" ht="15" thickBot="1">
+      <c r="A2" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="E2" s="14">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G2" s="23">
+        <v>1001</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J2" s="23">
+        <v>1</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L2" s="23">
+        <v>500</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N2" s="23">
+        <v>100</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="P2" s="23">
+        <v>300</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="R2" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" thickBot="1">
+      <c r="A3" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="E3" s="14">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G3" s="23">
+        <v>1001</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J3" s="23">
+        <v>1</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L3" s="23">
+        <v>100</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N3" s="23">
+        <v>100</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="P3" s="23">
+        <v>300</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="R3" s="23">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" thickBot="1">
+      <c r="A4" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E4" s="14">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="G4" s="23">
+        <v>1001</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="J4" s="23">
+        <v>1</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="L4" s="23">
+        <v>100</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="N4" s="23">
+        <v>100</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="P4" s="23">
+        <v>500</v>
+      </c>
+      <c r="Q4" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="R4" s="23">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T142"/>
   <sheetViews>

</xml_diff>